<commit_message>
hardware: fabrication: Generating again fabrication files after last DRC check #47
</commit_message>
<xml_diff>
--- a/hardware/fabrication/board_bom_ttc2.xlsx
+++ b/hardware/fabrication/board_bom_ttc2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yan Azeredo\Desktop\SpaceLab\ttc2\hardware\fabrication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B71FC7-538D-4A50-94FA-9364D4D4289A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA67B1A-9001-41F0-80CF-376A381B2B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
     <t>6/15/2021</t>
   </si>
   <si>
-    <t>5:03:08 PM</t>
+    <t>5:35:21 PM</t>
   </si>
   <si>
     <t>Designator</t>
@@ -1239,8 +1239,8 @@
   </sheetPr>
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="F7" s="8">
         <f ca="1">NOW()</f>
-        <v>44362.711815625</v>
+        <v>44362.734149189811</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>

</xml_diff>